<commit_message>
update reference update demo Add: Template and parameter marker attribute Add: Data validation
</commit_message>
<xml_diff>
--- a/demo/Demo.xlsx
+++ b/demo/Demo.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9825" windowHeight="4560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,42 +24,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>TYPE</t>
   </si>
   <si>
+    <t>STOCK</t>
+  </si>
+  <si>
     <t>NAME</t>
   </si>
   <si>
+    <t>PRICE</t>
+  </si>
+  <si>
+    <t>MU</t>
+  </si>
+  <si>
+    <t>SIGMA</t>
+  </si>
+  <si>
+    <t>DIVIDEND</t>
+  </si>
+  <si>
     <t>ID</t>
   </si>
   <si>
-    <t>METHOD</t>
-  </si>
-  <si>
-    <t>RESULT</t>
-  </si>
-  <si>
-    <t>FUNC</t>
-  </si>
-  <si>
-    <t>STOCK</t>
-  </si>
-  <si>
-    <t>PRICE</t>
-  </si>
-  <si>
-    <t>MU</t>
-  </si>
-  <si>
-    <t>SIGMA</t>
-  </si>
-  <si>
-    <t>DIVIDEND</t>
-  </si>
-  <si>
-    <t>EUROCALLOPTION</t>
+    <t>EUROSTOCKOPTION</t>
   </si>
   <si>
     <t>STRIKE</t>
@@ -71,44 +62,66 @@
     <t>UNDERLYING</t>
   </si>
   <si>
-    <t>CHECKUNDERLYING</t>
-  </si>
-  <si>
-    <t>EUROCALLPRICING</t>
-  </si>
-  <si>
-    <t>OPTION</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>SUB</t>
-  </si>
-  <si>
-    <t>BISEARCH</t>
-  </si>
-  <si>
-    <t>TARGET</t>
-  </si>
-  <si>
-    <t>LOWER</t>
-  </si>
-  <si>
-    <t>UPPER</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>X</t>
+    <t>OPTIONTYPE</t>
+  </si>
+  <si>
+    <t>CALL</t>
   </si>
   <si>
     <t>AAPL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Call500</t>
+    <t>AAPL_ATM_OP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>METHOD</t>
+  </si>
+  <si>
+    <t>CHECKUNDERLYING</t>
+  </si>
+  <si>
+    <t>RESULT</t>
+  </si>
+  <si>
+    <t>FUNC</t>
+  </si>
+  <si>
+    <t>EUROOPTIONPRICING</t>
+  </si>
+  <si>
+    <t>OPTION</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>SUB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BISEARCH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TARGET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOWER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPPER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -206,7 +219,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -226,6 +239,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -508,207 +527,436 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O8"/>
+  <dimension ref="B2:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.75" style="7"/>
+    <col min="2" max="2" width="9.75" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.25" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.75" style="7"/>
+    <col min="5" max="5" width="12.75" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.75" style="7"/>
+    <col min="8" max="8" width="9" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.75" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.75" style="7"/>
+    <col min="11" max="12" width="16" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.25" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="2.75" style="7"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="4" t="str">
+        <f ca="1">F8</f>
+        <v>⚓ AAPL_ATM_OP</v>
+      </c>
+      <c r="K2" s="8" t="str">
+        <f t="array" aca="1" ref="K2:M5" ca="1">_xll.ViewCache()</f>
+        <v>ID</v>
+      </c>
+      <c r="L2" s="8" t="str">
+        <f ca="1"/>
+        <v>TYPE</v>
+      </c>
+      <c r="M2" s="8" t="str">
+        <f ca="1"/>
+        <v>INIT</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="4" t="str">
-        <f ca="1">F7</f>
-        <v>⚓ Call500</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="5" t="s">
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="8" t="str">
+        <f ca="1"/>
+        <v>⚓ AAPL_ATM_OP</v>
+      </c>
+      <c r="L3" s="8" t="str">
+        <f ca="1"/>
+        <v>EuroStockOption</v>
+      </c>
+      <c r="M3" s="8" t="str">
+        <f ca="1"/>
+        <v>[Demo.xlsx]Sheet1!$F$8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="2" t="str">
-        <f ca="1">F7</f>
-        <v>⚓ Call500</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O3" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="C4" s="2">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F4" s="2">
-        <v>500</v>
+        <f>C4</f>
+        <v>100</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="I4" s="3" t="str">
         <f t="array" aca="1" ref="I4" ca="1">_xll.TempCall(H2:I3)</f>
         <v>⚓ AAPL</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="K4" s="8" t="str">
+        <f ca="1"/>
+        <v>⚓ AAPL</v>
+      </c>
+      <c r="L4" s="8" t="str">
+        <f ca="1"/>
+        <v>Stock</v>
+      </c>
+      <c r="M4" s="8" t="str">
+        <f ca="1"/>
+        <v>[Demo.xlsx]Sheet1!$C$8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F5" s="2">
-        <v>1</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L5" s="3">
-        <f t="array" aca="1" ref="L5" ca="1">_xll.TempCall(K2:L4)</f>
-        <v>50.000000604719958</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="K5" s="8" t="str">
+        <f ca="1"/>
+        <v>--</v>
+      </c>
+      <c r="L5" s="8" t="str">
+        <f ca="1"/>
+        <v>--</v>
+      </c>
+      <c r="M5" s="8" t="str">
+        <f ca="1"/>
+        <v>--</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2">
-        <f>O7</f>
-        <v>0.23029403761029243</v>
+        <f>I16</f>
+        <v>0.2407408095896244</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F6" s="2" t="str">
         <f ca="1">C8</f>
         <v>⚓ AAPL</v>
       </c>
-      <c r="N6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O6" s="2">
-        <f ca="1">L5</f>
-        <v>50.000000604719958</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="H6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2">
         <v>0.01</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="3" t="str">
-        <f t="array" aca="1" ref="F7" ca="1">_xll.TempCall(E2:F6)</f>
-        <v>⚓ Call500</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O7" s="2">
-        <v>0.23029403761029243</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="E7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="2" t="str">
+        <f ca="1">F8</f>
+        <v>⚓ AAPL_ATM_OP</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3" t="str">
         <f t="array" aca="1" ref="C8" ca="1">_xll.TempCall(B2:C7)</f>
         <v>⚓ AAPL</v>
       </c>
+      <c r="E8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="3" t="str">
+        <f t="array" aca="1" ref="F8" ca="1">_xll.TempCall(E2:F7)</f>
+        <v>⚓ AAPL_ATM_OP</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="H9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="array" aca="1" ref="I9" ca="1">_xll.TempCall(H6:I8)</f>
+        <v>15.000000070835782</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B10" s="8" t="str">
+        <f t="array" aca="1" ref="B10:C16" ca="1">_xll.ViewObject(C8)</f>
+        <v>ID</v>
+      </c>
+      <c r="C10" s="8" t="str">
+        <f ca="1"/>
+        <v>⚓ AAPL</v>
+      </c>
+      <c r="E10" s="8" t="str">
+        <f t="array" aca="1" ref="E10:F16" ca="1">_xll.ViewObject(F8)</f>
+        <v>ID</v>
+      </c>
+      <c r="F10" s="8" t="str">
+        <f ca="1"/>
+        <v>⚓ AAPL_ATM_OP</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B11" s="8" t="str">
+        <f ca="1"/>
+        <v>TYPE</v>
+      </c>
+      <c r="C11" s="8" t="str">
+        <f ca="1"/>
+        <v>Stock</v>
+      </c>
+      <c r="E11" s="8" t="str">
+        <f ca="1"/>
+        <v>TYPE</v>
+      </c>
+      <c r="F11" s="8" t="str">
+        <f ca="1"/>
+        <v>EuroStockOption</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B12" s="8" t="str">
+        <f ca="1"/>
+        <v>INIT</v>
+      </c>
+      <c r="C12" s="8" t="str">
+        <f ca="1"/>
+        <v>[Demo.xlsx]Sheet1!$C$8</v>
+      </c>
+      <c r="E12" s="8" t="str">
+        <f ca="1"/>
+        <v>INIT</v>
+      </c>
+      <c r="F12" s="8" t="str">
+        <f ca="1"/>
+        <v>[Demo.xlsx]Sheet1!$F$8</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="2">
+        <f ca="1">I9</f>
+        <v>15.000000070835782</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B13" s="8" t="str">
+        <f ca="1"/>
+        <v>PRICE</v>
+      </c>
+      <c r="C13" s="8">
+        <f ca="1"/>
+        <v>100</v>
+      </c>
+      <c r="E13" s="8" t="str">
+        <f ca="1"/>
+        <v>STRIKE</v>
+      </c>
+      <c r="F13" s="8">
+        <f ca="1"/>
+        <v>100</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B14" s="8" t="str">
+        <f ca="1"/>
+        <v>MU</v>
+      </c>
+      <c r="C14" s="8">
+        <f ca="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="E14" s="8" t="str">
+        <f ca="1"/>
+        <v>MATURITY</v>
+      </c>
+      <c r="F14" s="8">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B15" s="8" t="str">
+        <f ca="1"/>
+        <v>SIGMA</v>
+      </c>
+      <c r="C15" s="8">
+        <f ca="1"/>
+        <v>0.2407408095896244</v>
+      </c>
+      <c r="E15" s="8" t="str">
+        <f ca="1"/>
+        <v>UNDERLYING</v>
+      </c>
+      <c r="F15" s="8" t="str">
+        <f ca="1"/>
+        <v>⚓ AAPL</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B16" s="8" t="str">
+        <f ca="1"/>
+        <v>DIVIDEND</v>
+      </c>
+      <c r="C16" s="8">
+        <f ca="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="E16" s="8" t="str">
+        <f ca="1"/>
+        <v>OPTIONTYPE</v>
+      </c>
+      <c r="F16" s="8" t="str">
+        <f ca="1"/>
+        <v>CALL</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0.2407408095896244</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="21">
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="SharpObj STOCK" prompt="Stock prompt" sqref="C2"/>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter NAME: String" prompt="Unique SharpObj ID in this Excel workbook_x000d__x000a__x000d__x000a_- Input must be String" sqref="C3 F3"/>
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter PRICE: Double" prompt="Current stock price_x000d__x000a__x000d__x000a_- Input must between 0 and 1E+100" sqref="C4">
+      <formula1>0</formula1>
+      <formula2>1E+100</formula2>
+    </dataValidation>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter MU: Double" prompt="Mean return_x000d__x000a__x000d__x000a_- Input must be Double" sqref="C5"/>
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter SIGMA: Double" prompt="Volatility_x000d__x000a__x000d__x000a_- Input must between 0 and 1" sqref="C6">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter DIVIDEND: Double" prompt="Dividend yield_x000d__x000a__x000d__x000a_- Input must between 0 and 1" sqref="C7">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="SharpObj EUROSTOCKOPTION" prompt="European option" sqref="F2"/>
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter STRIKE: Double" prompt="Strike price_x000d__x000a__x000d__x000a_- Input must between 0 and 1E+100" sqref="F4">
+      <formula1>0</formula1>
+      <formula2>1E+100</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter MATURITY: Double" prompt="Time to maturity_x000d__x000a__x000d__x000a_- Input must between 0 and 1E+100" sqref="F5">
+      <formula1>0</formula1>
+      <formula2>1E+100</formula2>
+    </dataValidation>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter UNDERLYING: Stock" prompt="Underlying_x000d__x000a__x000d__x000a_- Input must be valid Stock ID" sqref="F6"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter OPTIONTYPE: OptionType" prompt="Option type_x000d__x000a__x000d__x000a_- Input must be selected from [CALL, PUT]" sqref="F7">
+      <formula1>"CALL, PUT"</formula1>
+    </dataValidation>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="STOCKOPTION.CHECKUNDERLYING" prompt="Show the underlying of a option" sqref="I3"/>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="function EUROOPTIONPRICING" prompt="Calculate price by BSM" sqref="I6"/>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter OPTION: StockOption" prompt="Option to be calculated_x000d__x000a__x000d__x000a_- Input must be valid StockOption ID" sqref="I7"/>
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter R: Double" prompt="Risk free rate to be used_x000d__x000a__x000d__x000a_- Input must between -1 and 1" sqref="I8">
+      <formula1>-1</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="subroutine BISEARCH" prompt="Solve a monotone equation" sqref="I11"/>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter Y: formula" prompt="Dependent variable" sqref="I12"/>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter TARGET: Double" prompt="Target value for y to reach_x000d__x000a__x000d__x000a_- Input must be Double" sqref="I13"/>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter LOWER: Double" prompt="Lower bound_x000d__x000a__x000d__x000a_- Input must be Double" sqref="I14"/>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter UPPER: Double" prompt="Upper bound_x000d__x000a__x000d__x000a_- Input must be Double" sqref="I15"/>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter X: placeholder" prompt="Independent variable" sqref="I16"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update reference change: Parameter attributes
</commit_message>
<xml_diff>
--- a/demo/Demo.xlsx
+++ b/demo/Demo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>TYPE</t>
   </si>
@@ -48,80 +48,83 @@
   </si>
   <si>
     <t>ID</t>
-  </si>
-  <si>
-    <t>EUROSTOCKOPTION</t>
-  </si>
-  <si>
-    <t>STRIKE</t>
-  </si>
-  <si>
-    <t>MATURITY</t>
-  </si>
-  <si>
-    <t>UNDERLYING</t>
-  </si>
-  <si>
-    <t>OPTIONTYPE</t>
-  </si>
-  <si>
-    <t>CALL</t>
   </si>
   <si>
     <t>AAPL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>AAPL_ATM_OP</t>
+    <t>EUROSTOCKOPTION</t>
+  </si>
+  <si>
+    <t>STRIKE</t>
+  </si>
+  <si>
+    <t>MATURITY</t>
+  </si>
+  <si>
+    <t>UNDERLYING</t>
+  </si>
+  <si>
+    <t>OPTIONTYPE</t>
+  </si>
+  <si>
+    <t>CALL</t>
+  </si>
+  <si>
+    <t>AAPL_ATM</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>RESULT</t>
+  </si>
+  <si>
+    <t>FUNC</t>
+  </si>
+  <si>
+    <t>EUROOPTIONPRICING</t>
+  </si>
+  <si>
+    <t>OPTION</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>SUB</t>
+  </si>
+  <si>
+    <t>BISEARCH</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>TARGET</t>
+  </si>
+  <si>
+    <t>LOWER</t>
+  </si>
+  <si>
+    <t>UPPER</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>METHOD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>CHECKUNDERLYING</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>RESULT</t>
-  </si>
-  <si>
-    <t>FUNC</t>
-  </si>
-  <si>
-    <t>EUROOPTIONPRICING</t>
-  </si>
-  <si>
-    <t>OPTION</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>SUB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BISEARCH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TARGET</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LOWER</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UPPER</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>X</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -219,7 +222,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -239,12 +242,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -530,24 +527,20 @@
   <dimension ref="B2:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.75" style="7"/>
-    <col min="2" max="2" width="9.75" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.25" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.75" style="7"/>
-    <col min="5" max="5" width="12.75" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.75" style="7"/>
-    <col min="8" max="8" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.75" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.75" style="7"/>
-    <col min="11" max="12" width="16" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.25" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="2.75" style="7"/>
+    <col min="2" max="2" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.2">
@@ -561,24 +554,24 @@
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="I2" s="4" t="str">
         <f ca="1">F8</f>
-        <v>⚓ AAPL_ATM_OP</v>
-      </c>
-      <c r="K2" s="8" t="str">
+        <v>⚓ AAPL_ATM</v>
+      </c>
+      <c r="K2" s="2" t="str">
         <f t="array" aca="1" ref="K2:M5" ca="1">_xll.ViewCache()</f>
         <v>ID</v>
       </c>
-      <c r="L2" s="8" t="str">
+      <c r="L2" s="2" t="str">
         <f ca="1"/>
         <v>TYPE</v>
       </c>
-      <c r="M2" s="8" t="str">
+      <c r="M2" s="2" t="str">
         <f ca="1"/>
         <v>INIT</v>
       </c>
@@ -588,7 +581,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>2</v>
@@ -597,20 +590,20 @@
         <v>15</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="8" t="str">
-        <f ca="1"/>
-        <v>⚓ AAPL_ATM_OP</v>
-      </c>
-      <c r="L3" s="8" t="str">
+        <v>30</v>
+      </c>
+      <c r="K3" s="2" t="str">
+        <f ca="1"/>
+        <v>⚓ AAPL_ATM</v>
+      </c>
+      <c r="L3" s="2" t="str">
         <f ca="1"/>
         <v>EuroStockOption</v>
       </c>
-      <c r="M3" s="8" t="str">
+      <c r="M3" s="2" t="str">
         <f ca="1"/>
         <v>[Demo.xlsx]Sheet1!$F$8</v>
       </c>
@@ -623,28 +616,28 @@
         <v>100</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2">
         <f>C4</f>
         <v>100</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="I4" s="3" t="str">
         <f t="array" aca="1" ref="I4" ca="1">_xll.TempCall(H2:I3)</f>
         <v>⚓ AAPL</v>
       </c>
-      <c r="K4" s="8" t="str">
+      <c r="K4" s="2" t="str">
         <f ca="1"/>
         <v>⚓ AAPL</v>
       </c>
-      <c r="L4" s="8" t="str">
+      <c r="L4" s="2" t="str">
         <f ca="1"/>
         <v>Stock</v>
       </c>
-      <c r="M4" s="8" t="str">
+      <c r="M4" s="2" t="str">
         <f ca="1"/>
         <v>[Demo.xlsx]Sheet1!$C$8</v>
       </c>
@@ -654,23 +647,23 @@
         <v>4</v>
       </c>
       <c r="C5" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" s="2">
         <v>2</v>
       </c>
-      <c r="K5" s="8" t="str">
+      <c r="K5" s="2" t="str">
         <f ca="1"/>
         <v>--</v>
       </c>
-      <c r="L5" s="8" t="str">
+      <c r="L5" s="2" t="str">
         <f ca="1"/>
         <v>--</v>
       </c>
-      <c r="M5" s="8" t="str">
+      <c r="M5" s="2" t="str">
         <f ca="1"/>
         <v>--</v>
       </c>
@@ -681,20 +674,20 @@
       </c>
       <c r="C6" s="2">
         <f>I16</f>
-        <v>0.2407408095896244</v>
+        <v>0.24645281955599785</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F6" s="2" t="str">
         <f ca="1">C8</f>
         <v>⚓ AAPL</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
@@ -702,20 +695,20 @@
         <v>6</v>
       </c>
       <c r="C7" s="2">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I7" s="2" t="str">
         <f ca="1">F8</f>
-        <v>⚓ AAPL_ATM_OP</v>
+        <v>⚓ AAPL_ATM</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
@@ -731,192 +724,192 @@
       </c>
       <c r="F8" s="3" t="str">
         <f t="array" aca="1" ref="F8" ca="1">_xll.TempCall(E2:F7)</f>
-        <v>⚓ AAPL_ATM_OP</v>
+        <v>⚓ AAPL_ATM</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I8" s="2">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="H9" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I9" s="3">
         <f t="array" aca="1" ref="I9" ca="1">_xll.TempCall(H6:I8)</f>
-        <v>15.000000070835782</v>
+        <v>15.000000007402633</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B10" s="8" t="str">
+      <c r="B10" s="2" t="str">
         <f t="array" aca="1" ref="B10:C16" ca="1">_xll.ViewObject(C8)</f>
         <v>ID</v>
       </c>
-      <c r="C10" s="8" t="str">
+      <c r="C10" s="2" t="str">
         <f ca="1"/>
         <v>⚓ AAPL</v>
       </c>
-      <c r="E10" s="8" t="str">
+      <c r="E10" s="2" t="str">
         <f t="array" aca="1" ref="E10:F16" ca="1">_xll.ViewObject(F8)</f>
         <v>ID</v>
       </c>
-      <c r="F10" s="8" t="str">
-        <f ca="1"/>
-        <v>⚓ AAPL_ATM_OP</v>
+      <c r="F10" s="2" t="str">
+        <f ca="1"/>
+        <v>⚓ AAPL_ATM</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B11" s="8" t="str">
+      <c r="B11" s="2" t="str">
         <f ca="1"/>
         <v>TYPE</v>
       </c>
-      <c r="C11" s="8" t="str">
+      <c r="C11" s="2" t="str">
         <f ca="1"/>
         <v>Stock</v>
       </c>
-      <c r="E11" s="8" t="str">
+      <c r="E11" s="2" t="str">
         <f ca="1"/>
         <v>TYPE</v>
       </c>
-      <c r="F11" s="8" t="str">
+      <c r="F11" s="2" t="str">
         <f ca="1"/>
         <v>EuroStockOption</v>
       </c>
       <c r="H11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="str">
+        <f ca="1"/>
+        <v>INIT</v>
+      </c>
+      <c r="C12" s="2" t="str">
+        <f ca="1"/>
+        <v>[Demo.xlsx]Sheet1!$C$8</v>
+      </c>
+      <c r="E12" s="2" t="str">
+        <f ca="1"/>
+        <v>INIT</v>
+      </c>
+      <c r="F12" s="2" t="str">
+        <f ca="1"/>
+        <v>[Demo.xlsx]Sheet1!$F$8</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="8" t="str">
-        <f ca="1"/>
-        <v>INIT</v>
-      </c>
-      <c r="C12" s="8" t="str">
-        <f ca="1"/>
-        <v>[Demo.xlsx]Sheet1!$C$8</v>
-      </c>
-      <c r="E12" s="8" t="str">
-        <f ca="1"/>
-        <v>INIT</v>
-      </c>
-      <c r="F12" s="8" t="str">
-        <f ca="1"/>
-        <v>[Demo.xlsx]Sheet1!$F$8</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="I12" s="2">
         <f ca="1">I9</f>
-        <v>15.000000070835782</v>
+        <v>15.000000007402633</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="8" t="str">
+      <c r="B13" s="2" t="str">
         <f ca="1"/>
         <v>PRICE</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="2">
         <f ca="1"/>
         <v>100</v>
       </c>
-      <c r="E13" s="8" t="str">
+      <c r="E13" s="2" t="str">
         <f ca="1"/>
         <v>STRIKE</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="2">
         <f ca="1"/>
         <v>100</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I13" s="2">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="8" t="str">
+      <c r="B14" s="2" t="str">
         <f ca="1"/>
         <v>MU</v>
       </c>
-      <c r="C14" s="8">
-        <f ca="1"/>
-        <v>0.05</v>
-      </c>
-      <c r="E14" s="8" t="str">
+      <c r="C14" s="2">
+        <f ca="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="E14" s="2" t="str">
         <f ca="1"/>
         <v>MATURITY</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="2">
         <f ca="1"/>
         <v>2</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I14" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="8" t="str">
+      <c r="B15" s="2" t="str">
         <f ca="1"/>
         <v>SIGMA</v>
       </c>
-      <c r="C15" s="8">
-        <f ca="1"/>
-        <v>0.2407408095896244</v>
-      </c>
-      <c r="E15" s="8" t="str">
+      <c r="C15" s="2">
+        <f ca="1"/>
+        <v>0.24645281955599785</v>
+      </c>
+      <c r="E15" s="2" t="str">
         <f ca="1"/>
         <v>UNDERLYING</v>
       </c>
-      <c r="F15" s="8" t="str">
+      <c r="F15" s="2" t="str">
         <f ca="1"/>
         <v>⚓ AAPL</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I15" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B16" s="8" t="str">
+      <c r="B16" s="2" t="str">
         <f ca="1"/>
         <v>DIVIDEND</v>
       </c>
-      <c r="C16" s="8">
-        <f ca="1"/>
-        <v>0.01</v>
-      </c>
-      <c r="E16" s="8" t="str">
+      <c r="C16" s="2">
+        <f ca="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="E16" s="2" t="str">
         <f ca="1"/>
         <v>OPTIONTYPE</v>
       </c>
-      <c r="F16" s="8" t="str">
+      <c r="F16" s="2" t="str">
         <f ca="1"/>
         <v>CALL</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I16" s="3">
-        <v>0.2407408095896244</v>
+        <v>0.24645281955599785</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="21">
+  <dataValidations count="22">
     <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="SharpObj STOCK" prompt="Stock prompt" sqref="C2"/>
-    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter NAME: String" prompt="Unique SharpObj ID in this Excel workbook_x000d__x000a__x000d__x000a_- Input must be String" sqref="C3 F3"/>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter NAME: String" prompt="Input must be String" sqref="C3 F3"/>
     <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter PRICE: Double" prompt="Current stock price_x000d__x000a__x000d__x000a_- Input must between 0 and 1E+100" sqref="C4">
       <formula1>0</formula1>
       <formula2>1E+100</formula2>
@@ -943,7 +936,6 @@
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter OPTIONTYPE: OptionType" prompt="Option type_x000d__x000a__x000d__x000a_- Input must be selected from [CALL, PUT]" sqref="F7">
       <formula1>"CALL, PUT"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="STOCKOPTION.CHECKUNDERLYING" prompt="Show the underlying of a option" sqref="I3"/>
     <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="function EUROOPTIONPRICING" prompt="Calculate price by BSM" sqref="I6"/>
     <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter OPTION: StockOption" prompt="Option to be calculated_x000d__x000a__x000d__x000a_- Input must be valid StockOption ID" sqref="I7"/>
     <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter R: Double" prompt="Risk free rate to be used_x000d__x000a__x000d__x000a_- Input must between -1 and 1" sqref="I8">
@@ -953,9 +945,17 @@
     <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="subroutine BISEARCH" prompt="Solve a monotone equation" sqref="I11"/>
     <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter Y: formula" prompt="Dependent variable" sqref="I12"/>
     <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter TARGET: Double" prompt="Target value for y to reach_x000d__x000a__x000d__x000a_- Input must be Double" sqref="I13"/>
-    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter LOWER: Double" prompt="Lower bound_x000d__x000a__x000d__x000a_- Input must be Double" sqref="I14"/>
-    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter UPPER: Double" prompt="Upper bound_x000d__x000a__x000d__x000a_- Input must be Double" sqref="I15"/>
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter LOWER: Double" prompt="Lower bound_x000d__x000a__x000d__x000a_- Input must between -1E+100 and 1E+100" sqref="I14">
+      <formula1>-1E+100</formula1>
+      <formula2>1E+100</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter UPPER: Double" prompt="Upper bound_x000d__x000a__x000d__x000a_- Input must between -1E+100 and 1E+100" sqref="I15">
+      <formula1>-1E+100</formula1>
+      <formula2>1E+100</formula2>
+    </dataValidation>
     <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter X: placeholder" prompt="Independent variable" sqref="I16"/>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="ID: STOCKOPTION" prompt="Input must be valid STOCKOPTION ID" sqref="I2"/>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="STOCKOPTION.CHECKUNDERLYING" prompt="Show the underlying of a option" sqref="I3"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update reference add: current object selection drop-down add: Ribbon tool
</commit_message>
<xml_diff>
--- a/demo/Demo.xlsx
+++ b/demo/Demo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>TYPE</t>
   </si>
@@ -72,10 +72,6 @@
     <t>CALL</t>
   </si>
   <si>
-    <t>AAPL_ATM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>RESULT</t>
   </si>
   <si>
@@ -126,6 +122,12 @@
   <si>
     <t>RESULT</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>⚓ AAPL_ATM</t>
+  </si>
+  <si>
+    <t>AAPL_ATM</t>
   </si>
 </sst>
 </file>
@@ -527,7 +529,7 @@
   <dimension ref="B2:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -557,11 +559,10 @@
         <v>9</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="4" t="str">
-        <f ca="1">F8</f>
-        <v>⚓ AAPL_ATM</v>
+        <v>27</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="K2" s="2" t="str">
         <f t="array" aca="1" ref="K2:M5" ca="1">_xll.ViewCache()</f>
@@ -587,13 +588,13 @@
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="H3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="K3" s="2" t="str">
         <f ca="1"/>
@@ -623,7 +624,7 @@
         <v>100</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4" s="3" t="str">
         <f t="array" aca="1" ref="I4" ca="1">_xll.TempCall(H2:I3)</f>
@@ -684,10 +685,10 @@
         <v>⚓ AAPL</v>
       </c>
       <c r="H6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
@@ -704,11 +705,10 @@
         <v>14</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="2" t="str">
-        <f ca="1">F8</f>
-        <v>⚓ AAPL_ATM</v>
+        <v>18</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
@@ -727,7 +727,7 @@
         <v>⚓ AAPL_ATM</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I8" s="2">
         <v>0.04</v>
@@ -735,7 +735,7 @@
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="H9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I9" s="3">
         <f t="array" aca="1" ref="I9" ca="1">_xll.TempCall(H6:I8)</f>
@@ -778,10 +778,10 @@
         <v>EuroStockOption</v>
       </c>
       <c r="H11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.2">
@@ -802,7 +802,7 @@
         <v>[Demo.xlsx]Sheet1!$F$8</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I12" s="2">
         <f ca="1">I9</f>
@@ -827,7 +827,7 @@
         <v>100</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I13" s="2">
         <v>15</v>
@@ -851,7 +851,7 @@
         <v>2</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I14" s="2">
         <v>0</v>
@@ -875,7 +875,7 @@
         <v>⚓ AAPL</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I15" s="2">
         <v>1</v>
@@ -899,7 +899,7 @@
         <v>CALL</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I16" s="3">
         <v>0.24645281955599785</v>
@@ -937,7 +937,6 @@
       <formula1>"CALL, PUT"</formula1>
     </dataValidation>
     <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="function EUROOPTIONPRICING" prompt="Calculate price by BSM" sqref="I6"/>
-    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter OPTION: StockOption" prompt="Option to be calculated_x000d__x000a__x000d__x000a_- Input must be valid StockOption ID" sqref="I7"/>
     <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter R: Double" prompt="Risk free rate to be used_x000d__x000a__x000d__x000a_- Input must between -1 and 1" sqref="I8">
       <formula1>-1</formula1>
       <formula2>1</formula2>
@@ -954,8 +953,13 @@
       <formula2>1E+100</formula2>
     </dataValidation>
     <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter X: placeholder" prompt="Independent variable" sqref="I16"/>
-    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="ID: STOCKOPTION" prompt="Input must be valid STOCKOPTION ID" sqref="I2"/>
     <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="STOCKOPTION.CHECKUNDERLYING" prompt="Show the underlying of a option" sqref="I3"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="EUROSTOCKOPTION selection" prompt="Current objects with type EUROSTOCKOPTION_x000d__x000a__x000d__x000a_- Input must be selected from [⚓ AAPL_ATM]" sqref="I2">
+      <formula1>"⚓ AAPL_ATM"</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="EUROSTOCKOPTION selection" prompt="Current objects with type EUROSTOCKOPTION_x000d__x000a__x000d__x000a_- Input must be selected from [⚓ AAPL_ATM]" sqref="I7">
+      <formula1>"⚓ AAPL_ATM"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update reference add: sub can get initial value of action by using ActionSet<T>.Initial add: data table and data array support
</commit_message>
<xml_diff>
--- a/demo/Demo.xlsx
+++ b/demo/Demo.xlsx
@@ -87,47 +87,54 @@
     <t>R</t>
   </si>
   <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>METHOD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHECKUNDERLYING</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RESULT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>⚓ AAPL_ATM</t>
+  </si>
+  <si>
+    <t>AAPL_ATM</t>
+  </si>
+  <si>
     <t>SUB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>BISEARCH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TARGET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOWER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPPER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>TARGET</t>
-  </si>
-  <si>
-    <t>LOWER</t>
-  </si>
-  <si>
-    <t>UPPER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>X</t>
-  </si>
-  <si>
-    <t>ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>METHOD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CHECKUNDERLYING</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RESULT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>⚓ AAPL_ATM</t>
-  </si>
-  <si>
-    <t>AAPL_ATM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -559,10 +566,10 @@
         <v>9</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="K2" s="2" t="str">
         <f t="array" aca="1" ref="K2:M5" ca="1">_xll.ViewCache()</f>
@@ -588,13 +595,13 @@
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="K3" s="2" t="str">
         <f ca="1"/>
@@ -624,7 +631,7 @@
         <v>100</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="I4" s="3" t="str">
         <f t="array" aca="1" ref="I4" ca="1">_xll.TempCall(H2:I3)</f>
@@ -674,7 +681,6 @@
         <v>5</v>
       </c>
       <c r="C6" s="2">
-        <f>I16</f>
         <v>0.24645281955599785</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -708,7 +714,7 @@
         <v>18</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
@@ -778,10 +784,10 @@
         <v>EuroStockOption</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.2">
@@ -802,85 +808,85 @@
         <v>[Demo.xlsx]Sheet1!$F$8</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="I12" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="str">
+        <f ca="1"/>
+        <v>PRICE</v>
+      </c>
+      <c r="C13" s="2">
+        <f ca="1"/>
+        <v>100</v>
+      </c>
+      <c r="E13" s="2" t="str">
+        <f ca="1"/>
+        <v>STRIKE</v>
+      </c>
+      <c r="F13" s="2">
+        <f ca="1"/>
+        <v>100</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="str">
+        <f ca="1"/>
+        <v>MU</v>
+      </c>
+      <c r="C14" s="2">
+        <f ca="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="E14" s="2" t="str">
+        <f ca="1"/>
+        <v>MATURITY</v>
+      </c>
+      <c r="F14" s="2">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="str">
+        <f ca="1"/>
+        <v>SIGMA</v>
+      </c>
+      <c r="C15" s="2">
+        <f ca="1"/>
+        <v>0.24645281955599785</v>
+      </c>
+      <c r="E15" s="2" t="str">
+        <f ca="1"/>
+        <v>UNDERLYING</v>
+      </c>
+      <c r="F15" s="2" t="str">
+        <f ca="1"/>
+        <v>⚓ AAPL</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="2">
         <f ca="1">I9</f>
         <v>15.000000007402633</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="2" t="str">
-        <f ca="1"/>
-        <v>PRICE</v>
-      </c>
-      <c r="C13" s="2">
-        <f ca="1"/>
-        <v>100</v>
-      </c>
-      <c r="E13" s="2" t="str">
-        <f ca="1"/>
-        <v>STRIKE</v>
-      </c>
-      <c r="F13" s="2">
-        <f ca="1"/>
-        <v>100</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="str">
-        <f ca="1"/>
-        <v>MU</v>
-      </c>
-      <c r="C14" s="2">
-        <f ca="1"/>
-        <v>0.1</v>
-      </c>
-      <c r="E14" s="2" t="str">
-        <f ca="1"/>
-        <v>MATURITY</v>
-      </c>
-      <c r="F14" s="2">
-        <f ca="1"/>
-        <v>2</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="2" t="str">
-        <f ca="1"/>
-        <v>SIGMA</v>
-      </c>
-      <c r="C15" s="2">
-        <f ca="1"/>
-        <v>0.24645281955599785</v>
-      </c>
-      <c r="E15" s="2" t="str">
-        <f ca="1"/>
-        <v>UNDERLYING</v>
-      </c>
-      <c r="F15" s="2" t="str">
-        <f ca="1"/>
-        <v>⚓ AAPL</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I15" s="2">
-        <v>1</v>
-      </c>
-    </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="str">
         <f ca="1"/>
@@ -898,11 +904,12 @@
         <f ca="1"/>
         <v>CALL</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I16" s="3">
-        <v>0.24645281955599785</v>
+      <c r="H16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" s="2" t="str">
+        <f ca="1">_xll.Ref(C6)</f>
+        <v>⚓ SHEET1!$C$6</v>
       </c>
     </row>
   </sheetData>
@@ -941,18 +948,6 @@
       <formula1>-1</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="subroutine BISEARCH" prompt="Solve a monotone equation" sqref="I11"/>
-    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter Y: formula" prompt="Dependent variable" sqref="I12"/>
-    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter TARGET: Double" prompt="Target value for y to reach_x000d__x000a__x000d__x000a_- Input must be Double" sqref="I13"/>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter LOWER: Double" prompt="Lower bound_x000d__x000a__x000d__x000a_- Input must between -1E+100 and 1E+100" sqref="I14">
-      <formula1>-1E+100</formula1>
-      <formula2>1E+100</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter UPPER: Double" prompt="Upper bound_x000d__x000a__x000d__x000a_- Input must between -1E+100 and 1E+100" sqref="I15">
-      <formula1>-1E+100</formula1>
-      <formula2>1E+100</formula2>
-    </dataValidation>
-    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter X: placeholder" prompt="Independent variable" sqref="I16"/>
     <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="STOCKOPTION.CHECKUNDERLYING" prompt="Show the underlying of a option" sqref="I3"/>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="EUROSTOCKOPTION selection" prompt="Current objects with type EUROSTOCKOPTION_x000d__x000a__x000d__x000a_- Input must be selected from [⚓ AAPL_ATM]" sqref="I2">
       <formula1>"⚓ AAPL_ATM"</formula1>
@@ -960,6 +955,18 @@
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="EUROSTOCKOPTION selection" prompt="Current objects with type EUROSTOCKOPTION_x000d__x000a__x000d__x000a_- Input must be selected from [⚓ AAPL_ATM]" sqref="I7">
       <formula1>"⚓ AAPL_ATM"</formula1>
     </dataValidation>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="subroutine BISEARCH" prompt="Solve a monotone equation" sqref="I11"/>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter TARGET: Double" prompt="Target value for y to reach_x000d__x000a__x000d__x000a_- Input must be Double" sqref="I12"/>
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter LOWER: Double" prompt="Lower bound_x000d__x000a__x000d__x000a_- Input must between -1E+100 and 1E+100" sqref="I13">
+      <formula1>-1E+100</formula1>
+      <formula2>1E+100</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter UPPER: Double" prompt="Upper bound_x000d__x000a__x000d__x000a_- Input must between -1E+100 and 1E+100" sqref="I14">
+      <formula1>-1E+100</formula1>
+      <formula2>1E+100</formula2>
+    </dataValidation>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter Y: formula" prompt="Dependent variable" sqref="I15"/>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parameter X: placeholder" prompt="Independent variable_x000d__x000a__x000d__x000a_- Either a reference to target cell, or let target cell equal to this cell" sqref="I16"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>